<commit_message>
Make cell format storage column major.
</commit_message>
<xml_diff>
--- a/test/xlsx/formatted-text/bold-and-italic.xlsx
+++ b/test/xlsx/formatted-text/bold-and-italic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="28695" windowHeight="12780"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="18225" windowHeight="12000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Normal Text</t>
   </si>
@@ -28,6 +28,50 @@
   </si>
   <si>
     <t>Bold and Italic Text</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bold</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Italic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> mixed</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -387,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -418,6 +462,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>